<commit_message>
added better parsing of dates
</commit_message>
<xml_diff>
--- a/tests/data/pbmc_shipping.xlsx
+++ b/tests/data/pbmc_shipping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-prism/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/schemas/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="4480" windowWidth="42200" windowHeight="23380"/>
+    <workbookView xWindow="3880" yWindow="4100" windowWidth="42200" windowHeight="23380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
   <si>
     <t>SHIPPING MANIFEST FOR PBMC SAMPLES</t>
   </si>
@@ -261,9 +261,6 @@
     <t>e</t>
   </si>
   <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>q</t>
   </si>
   <si>
@@ -280,15 +277,6 @@
   </si>
   <si>
     <t>sdsfd</t>
-  </si>
-  <si>
-    <t>sgs</t>
-  </si>
-  <si>
-    <t>sdfs</t>
-  </si>
-  <si>
-    <t>fsdhdf</t>
   </si>
   <si>
     <t>Endoscopic Biopsy</t>
@@ -412,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -429,6 +417,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,7 +726,7 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -886,8 +879,8 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>77</v>
+      <c r="B15" s="6">
+        <v>35797.806979166664</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -898,7 +891,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -931,7 +924,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -942,7 +935,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -987,13 +980,13 @@
         <v>23</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>26</v>
@@ -1070,10 +1063,10 @@
         <v>24</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>25</v>
@@ -1147,49 +1140,49 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
         <v>80</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" t="s">
+        <v>80</v>
+      </c>
+      <c r="I25" s="7">
+        <v>43417</v>
+      </c>
+      <c r="J25" s="8">
+        <v>0.84767361111111106</v>
+      </c>
+      <c r="K25" s="7">
+        <v>43417</v>
+      </c>
+      <c r="L25" s="8">
+        <v>0.84767361111111106</v>
+      </c>
+      <c r="M25" t="s">
         <v>81</v>
       </c>
-      <c r="C25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="N25" t="s">
         <v>83</v>
       </c>
-      <c r="H25" t="s">
-        <v>81</v>
-      </c>
-      <c r="I25" t="s">
-        <v>81</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="O25" t="s">
         <v>84</v>
-      </c>
-      <c r="K25" t="s">
-        <v>85</v>
-      </c>
-      <c r="L25" t="s">
-        <v>86</v>
-      </c>
-      <c r="M25" t="s">
-        <v>82</v>
-      </c>
-      <c r="N25" t="s">
-        <v>87</v>
-      </c>
-      <c r="O25" t="s">
-        <v>88</v>
       </c>
       <c r="P25">
         <v>5</v>
@@ -1207,7 +1200,7 @@
         <v>66</v>
       </c>
       <c r="U25" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="V25">
         <v>12364</v>
@@ -1219,13 +1212,13 @@
         <v>2222</v>
       </c>
       <c r="Y25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="Z25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="AA25" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>